<commit_message>
Made sure that the Excel output only contains cells that contain data Added a schema for the Excel output
</commit_message>
<xml_diff>
--- a/ms-office/xplmod/excel.mod/test/test.xlsx
+++ b/ms-office/xplmod/excel.mod/test/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Erik\xmldev\xtpxlib2\ms-office\xplmod\excel-to-xml.mod\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Erik\xmldev\xtpxlib2\ms-office\xplmod\excel.mod\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="19968" windowHeight="5136" activeTab="2"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="19968" windowHeight="5136"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,61 @@
     <definedName name="YEAR" localSheetId="1">'Blad1 (2)'!$A$2</definedName>
     <definedName name="YEAR">Blad1!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Erik Siegel</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Erik Siegel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Commentaar </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yeah</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> !!!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -164,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +273,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -611,10 +690,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -725,13 +806,21 @@
       <c r="C16" t="s">
         <v>19</v>
       </c>
+      <c r="F16">
+        <f>SUM(G16:K16)</f>
+        <v>5</v>
+      </c>
       <c r="G16" s="6">
         <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -864,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>